<commit_message>
Data Driven Automation Using Excel
</commit_message>
<xml_diff>
--- a/TestData/Deposit_Calculator.xlsx
+++ b/TestData/Deposit_Calculator.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gowri\GowriShankar_WorkSpace\SeleniumWebDriverPractice\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8029B1-1F53-4A4A-89BC-D4B13AA8F171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D67D3E-6C6D-4CA4-B256-97A97BE1DDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Initial Deposit Amount</t>
   </si>
@@ -58,12 +58,19 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,18 +418,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.08984375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="12" style="4" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="20.54296875"/>
+    <col min="2" max="2" customWidth="true" style="4" width="15.6328125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="11.453125"/>
+    <col min="4" max="4" customWidth="true" style="4" width="21.08984375"/>
+    <col min="5" max="5" customWidth="true" style="4" width="16.26953125"/>
+    <col min="6" max="6" customWidth="true" style="4" width="14.453125"/>
+    <col min="7" max="7" customWidth="true" style="4" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -467,7 +474,9 @@
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" t="s" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
@@ -488,7 +497,9 @@
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" t="s" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
@@ -509,7 +520,9 @@
       <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" t="s" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
@@ -530,7 +543,9 @@
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" t="s" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
@@ -551,7 +566,9 @@
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" t="s" s="4">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>